<commit_message>
pending run test cases with loops
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>CompleteFlowTestCase</t>
+  </si>
+  <si>
+    <t>NavigateFooterLinksTestCase</t>
   </si>
 </sst>
 </file>
@@ -99,7 +102,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -388,10 +391,10 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" customWidth="1"/>
@@ -433,7 +436,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -457,7 +460,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -469,7 +472,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>